<commit_message>
modify the command file
</commit_message>
<xml_diff>
--- a/GIT_Command.xlsx
+++ b/GIT_Command.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Command</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>push the changes to the center repository in github</t>
+  </si>
+  <si>
+    <t>$ git commit -am "comments"</t>
+  </si>
+  <si>
+    <t>directly commit changes from working area to repository. It skip staging area.</t>
   </si>
 </sst>
 </file>
@@ -428,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -536,6 +542,14 @@
         <v>23</v>
       </c>
     </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>